<commit_message>
special topic ins completed
</commit_message>
<xml_diff>
--- a/InputFiles/INS/TC01_INS_SpecialTopic-CancerMoonshot.xlsx
+++ b/InputFiles/INS/TC01_INS_SpecialTopic-CancerMoonshot.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radhakrishnang2/Desktop/Automation/gayathri26sep/Commons_Automation/InputFiles/INS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF238F1-84B1-4E4A-838B-A7F2EF2B25F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BDA0C4-9546-A947-8EC5-2B48BD2425B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17440" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="40080" yWindow="500" windowWidth="25800" windowHeight="17440" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,23 +65,6 @@
     <t>PublicationsTab</t>
   </si>
   <si>
-    <t>SELECT DISTINCT
-    COUNT(DISTINCT prg.program_id) AS "Programs",
-    COUNT(DISTINCT prj.project_id) AS "Projects",
-    COUNT(DISTINCT gnt.grant_id) AS "Grants",
-    COUNT(DISTINCT pub.pmid) AS "Publications"
-FROM 
-    df_program prg
-LEFT JOIN 
-    df_project prj ON prg.program_id = prj."program.program_id"
-LEFT JOIN 
-    df_grant gnt ON prj.project_id = gnt."project.project_id"
-LEFT JOIN 
-    df_publication pub ON prj.project_id = pub."project.project_id"
-WHERE 
-    prg.focus_area LIKE '%Cancer Moonshot%'</t>
-  </si>
-  <si>
     <t>TC01_INS_SpecialTopic-CancerMoonshot_TSVData.xlsx</t>
   </si>
   <si>
@@ -110,56 +93,6 @@
   </si>
   <si>
     <t>SELECT DISTINCT
-    gnt.grant_id AS "Grant ID", 
-    prj.project_id AS "Project",
-    gnt.grant_title AS "Grant Title",
-    gnt.principal_investigators AS "Principal Investigators",
-    gnt.program_officers AS "Program Officers",
-    gnt.fiscal_year AS "Fiscal Year",
-    gnt.project_end_date AS "Project End Date"
-FROM 
-    df_grant gnt
-LEFT JOIN 
-    df_project prj ON gnt."project.project_id" = prj.project_id
-LEFT JOIN 
-    df_program prg ON prj."program.program_id" = prg.program_id
-LEFT JOIN 
-    df_publication pub ON prj.project_id = pub."project.project_id"
-WHERE 
-    prg.focus_area LIKE '%Cancer Moonshot%'
-ORDER BY 
-    lower(gnt.grant_id) ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    pub.pmid AS "PubMed ID", 
-    pub.title AS "Title",
-    pub.authors AS "Authors",
-    pub.publication_date AS "Publication Date",
-    pub.cited_by AS "Cited By",
-    CASE 
-    WHEN pub.relative_citation_ratio = 0 THEN '0'
-    WHEN pub.relative_citation_ratio = 7.0 THEN '7'
-    WHEN pub.relative_citation_ratio = ROUND(pub.relative_citation_ratio) THEN CAST(ROUND(pub.relative_citation_ratio) AS VARCHAR) 
-    ELSE CAST(ROUND(pub.relative_citation_ratio, 2) AS VARCHAR)
-END AS "Relative Citation Ratio"
-FROM 
-    df_publication pub
-LEFT JOIN 
-    df_project prj ON pub."project.project_id" = prj.project_id
-LEFT JOIN 
-    df_program prg ON prj."program.program_id" = prg.program_id
-LEFT JOIN 
-    df_grant gnt ON prj.project_id = gnt."project.project_id"
-WHERE 
-    prg.focus_area LIKE '%Cancer Moonshot%'
-ORDER BY 
-    lower(pub.pmid) ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
     prj.project_id AS "Project ID", 
     prj.project_title AS "Project Title",
     prj.project_org_name AS "Organization",
@@ -179,28 +112,83 @@
     lower(prj.project_id) ASC
 LIMIT 100;</t>
   </si>
+  <si>
+    <t>SELECT DISTINCT
+    COUNT(DISTINCT prg.program_id) AS "Programs",
+    COUNT(DISTINCT prj.project_id) AS "Projects",
+    COUNT(DISTINCT gnt.grant_id) AS "Grants",
+    COUNT(DISTINCT pub.pmid) AS "Publications"
+FROM 
+    df_program prg
+LEFT JOIN 
+    df_project prj ON prg.program_id = prj."program.program_id"
+LEFT JOIN 
+    df_grant gnt ON prj.project_id = gnt."project.project_id"
+LEFT JOIN 
+    df_publication pub ON prj.project_id = pub."project.project_id"
+WHERE 
+    prg.focus_area LIKE '%Cancer Moonshot%';</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    gnt.grant_id AS "Grant ID", 
+    prj.project_id AS "Project",
+    gnt.grant_title AS "Grant Title",
+    gnt.principal_investigators AS "Principal Investigators",
+    gnt.program_officers AS "Program Officers",
+    gnt.fiscal_year AS "Fiscal Year",
+    gnt.grant_end_date AS "Project End Date"
+FROM 
+    df_grant gnt
+LEFT JOIN 
+    df_project prj ON gnt."project.project_id" = prj.project_id
+LEFT JOIN 
+    df_program prg ON prj."program.program_id" = prg.program_id
+LEFT JOIN 
+    df_publication pub ON prj.project_id = pub."project.project_id"
+WHERE 
+    prg.focus_area LIKE '%Cancer Moonshot%'
+ORDER BY 
+    lower(gnt.grant_id) ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    pub.pmid AS "PubMed ID", 
+    pub.publication_title AS "Title",
+    pub.authors AS "Authors",
+    pub.publication_date AS "Publication Date",
+    pub.cited_by AS "Cited By",
+    CASE 
+    WHEN pub.relative_citation_ratio = 0 THEN '0'
+    WHEN pub.relative_citation_ratio = 7.0 THEN '7'
+    WHEN pub.relative_citation_ratio = 1.0 THEN '1'
+    WHEN pub.relative_citation_ratio = 2.0 THEN '2'
+    WHEN pub.relative_citation_ratio = ROUND(pub.relative_citation_ratio) THEN CAST(ROUND(pub.relative_citation_ratio) AS VARCHAR) 
+    ELSE CAST(ROUND(pub.relative_citation_ratio, 2) AS VARCHAR)
+END AS "Relative Citation Ratio"
+FROM 
+    df_publication pub
+LEFT JOIN 
+    df_project prj ON pub."project.project_id" = prj.project_id
+LEFT JOIN 
+    df_program prg ON prj."program.program_id" = prg.program_id
+LEFT JOIN 
+    df_grant gnt ON prj.project_id = gnt."project.project_id"
+WHERE 
+    prg.focus_area LIKE '%Cancer Moonshot%'
+ORDER BY 
+    lower(pub.pmid) ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -253,17 +241,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -589,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -623,33 +605,33 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="187" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>15</v>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="356" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -657,8 +639,8 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>14</v>
+      <c r="B5" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -670,7 +652,7 @@
       <c r="C7" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>